<commit_message>
Submitted first task of the competition
</commit_message>
<xml_diff>
--- a/Data Devourers_IIMX.xlsx
+++ b/Data Devourers_IIMX.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5074" uniqueCount="5059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5075" uniqueCount="5060">
   <si>
     <t>ACCT_NUM</t>
   </si>
@@ -15171,36 +15171,39 @@
     <t>Used Regex in re library of Python and Pandas library for further processing to parse the required words. Regex code used to parse all the statements being - "[A-Z].+-Initial Level(.+)". Using this command - It obtained all the keywords from the customer statement seperated by "-". Then further split the string with delimiter "-", to obtain all the keywords in the list. Then, grouped the whole dataframe on the basis of accounts and took union of all those list (in same accounts as same person could do complaint more than once). Next, looped over the grouped dataframe (Used Apply method in Pandas) to change the elements in lists to either - "operation" (for Operation Capabilities), "payment" (for Payment Settlement), "utilit" (for Utilities/ Utility), "account" (for Account) ans simultaaneously counting their numbers and incrementing their value in dictionary of these 4 keywords.</t>
   </si>
   <si>
-    <t>Male tend to be more among churners than females.</t>
-  </si>
-  <si>
-    <t>More Churners are from North and East in comparrison to South and West.</t>
-  </si>
-  <si>
-    <t>People with middle lower salaries are most among Churners.</t>
-  </si>
-  <si>
-    <t>People of medium age - (30 - 60) are more among churners.</t>
-  </si>
-  <si>
-    <t>Those who have rented the equipment have more chnce of being Churner</t>
-  </si>
-  <si>
     <t>Those with valid address are more among Churners</t>
   </si>
   <si>
-    <t>Most Churners from Banking, Financial, Academic Sector</t>
-  </si>
-  <si>
     <t>Those with age of home less than 10 years are more among churners than those with age of home &gt; 10</t>
   </si>
   <si>
-    <t>First, we loaded the data in python using Pandas library. Then Seperated the Modelling and validation accounts for all the different data provided - Demo, Call Center, Default, Payment and Use Pattern data. Further we split the modelling data into training andtest dataset as we wanted to test the performance of our model on an untouched dataset. Pre-Processing :                             
+    <t>Assuming average age of marriage being 25, Married people are more among churners.</t>
+  </si>
+  <si>
+    <t>Male tend to be more among churners than females. But propotion of females who are Churner is more than males.</t>
+  </si>
+  <si>
+    <t>Most Churners are in age group of 50-60. But Maximum proportion of Churners in a particular age group is in 10-20.</t>
+  </si>
+  <si>
+    <t>More Churners are from North and East in comparison to South and West.</t>
+  </si>
+  <si>
+    <t>Those who have rented the equipment are more among Churners</t>
+  </si>
+  <si>
+    <t>Churners are most among those with salary range - [0,4] followed by [5-9] which is followed by [10-13]</t>
+  </si>
+  <si>
+    <t>Proportion of Churners is more among those with status - Closed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customers from Banking and Finance make upto 75% of Churners. </t>
+  </si>
+  <si>
+    <t>First, we loaded the data in python using Pandas library. Then Seperated the Modelling and validation accounts for all the different data provided - Demo, Call Center, Default, Payment and Use Pattern data. Further we split the modelling data into training and test dataset as we wanted to test the performance of our model on an untouched dataset. Pre-Processing :                             
 1. First took important featues from demographic data - Gender, Region, Age, Salary Slab, Professional Info, Age of home, Commence Date, Scheme, Churn Date.
-2. Then change feature - Churn date to Churner (0,1) depending on whether that customer left or not.                                                                                                                           3. Data is of year 2015. So changed the feature - "Commence date" to "Loyal Years of customer" whose value being - (2015 - commence year of customer).                                       4. Other features used for modelling from other data frames ( apart from Demographic Dataframe ) are - "Mean Sum paid in last three months", Complaints made in last 3 months - { "operation", "utility", "payment", "account" }. "Num of times customer was defaulter in last 3 months", "Mean Usage hours in last 3 months".                                                            5. Next, out of all these features Gender, Region, Professional Info, Scheme, Complaints (Customer statements) were the Nominal features and needed to modified properly. So new boolean features were formed i.e Region - {"North", "South", "East", "West"}, Gender - {"Male" -1, "female" - 0}, Complaints - {"operation", "utility", "payment", "account"}, Similarly for schemes and Prof Info also.                                                                                                                                                                                                                                                                   6. Out of all these correlation of these feature were checked to deal with curse of dimensionality. 2 features - "Average hours consumed" and 'Average payment made in last 3 months" were highly correlated. We just used "Average Payment made in last 3 months".                                                                                                                                                 7. We were left with 38 features + "Churner" + "Account Number". Next step we used was to deal with missing values. We imputed them using median.                                             Modelling :                                                                                                                                                                                                                                                                                  1. We now we have got 38 features and 1 target varible - "Churner" -  {0 - Non Churner, 1 - Churner}.                                                                                                                              2. We first used different machine learnng models - KNN, Logistic Regression, SVM - {RBF, Linear, Sigmoid}, Random Forest, Neural Networks. We made use K-Cross validation on our Training set with K = 10 to chose between different hyperparameters of different models with metric being AUC ( of ROC).                                                                                            3. Finally we tested the performance of these models with best hyperparameters on our hold out test set on the basis of AUC again.                                                                           4. Only Logistic Regression and Neural Networks performed quite well with AUC ~ 0.71.                                                                                                                                                     5. We calculated their probability of belonging to class - 1 through predefined functions in scikit learn library of Python. Next we had to chose a threshold. Clearly we want our sensitivity to be high and can somewhat compromise on specificity (but still not too low) because we want to focus on Churners and try to hold them with us. So we chosed the threshold based on maximum F1-Score.                                                                                                                                                                                                                               6. We then finally pre-processed our validation dataset as mentioned above and applied the models - Neural Network and Logistic Regression. My solution is on the basis of Neural Networks as it provied us with more number of churners and is somewhat more complicated than logistic regression.                                                                                      Tools : - Python ( Pandas - Data Processing, sklearn - ML, matplotlib - visualizations, Numpy - Basic array operations ), Excel ( Basic Understanding (Solution 1) and visualizations )</t>
-  </si>
-  <si>
-    <t>Assuming average age of marriage being 25, Married people are more among churners.</t>
+2. Then change feature - Churn date to Churner (0,1) depending on whether that customer left or not.                                                                                                                           3. Data is of year 2015. So changed the feature - "Commence date" to "Loyal Years of customer" whose value being - (2015 - commence year of customer).                                       4. Other features used for modelling from other data frames ( apart from Demographic Dataframe ) are - "Mean Sum paid in last three months", Complaints made in last 3 months - { "operation", "utility", "payment", "account" }. "Num of times customer was defaulter in last 3 months", "Mean Usage hours in last 3 months".                                                            5. Next, out of all these features Gender, Region, Professional Info, Scheme, Complaints (Customer statements) were the Nominal features and needed to modified properly. So new boolean features were formed i.e Region - {"North", "South", "East", "West"}, Gender - {"Male" -1, "female" - 0}, Complaints - {"operation", "utility", "payment", "account"}, Similarly for schemes and Prof Info also.                                                                                                                                                                                                                                                                   6. Out of all these correlation of these feature were checked to deal with curse of dimensionality. 2 features - "Average hours consumed" and 'Average payment made in last 3 months" were highly correlated. We just used "Average Payment made in last 3 months".                                                                                                                                                 7. We were left with 38 features + "Churner" + "Account Number". Next step we used was to deal with missing values. We imputed them using median.                                             Modelling :                                                                                                                                                                                                                                                                                  1. We now we have got 38 features and 1 target varible - "Churner" -  {0 - Non Churner, 1 - Churner}.                                                                                                                              2. We first used different machine learnng models - KNN, Logistic Regression, SVM - {RBF, Linear, Sigmoid}, Random Forest, Neural Networks. We made use of K-Cross validation on our Training set with K = 10 to chose between different hyperparameters of different models with metric being AUC ( of ROC).                                                                                            3. Finally we tested the performance of these models with best hyperparameters on our hold out test set on the basis of AUC again.                                                                           4. Only Logistic Regression and Neural Networks performed well enough with AUC ~ 0.71.                                                                                                                                                     5. We calculated their probability of belonging to class - 1 through predefined functions in scikit learn library of Python. Next we had to chose a threshold. Clearly we want our sensitivity to be high and can somewhat compromise on specificity (but still not too low) because we want to focus on Churners and try to hold them with us. So we chosed the threshold based on maximum F1-Score.                                                                                                                                                                                                                               6. We then finally pre-processed our validation dataset as mentioned above and applied the models - Neural Network and Logistic Regression. My solution is on the basis of 3 layered (2 hidden layers) Neural Networks as it provied us with more number of churners and is somewhat more complicated than logistic regression.                                                                                      Tools : - Python ( Pandas - Data Processing, sklearn - ML, matplotlib - visualizations, Numpy - Basic array operations ), Excel ( Basic Understanding (Solution 1) and visualizations )</t>
   </si>
 </sst>
 </file>
@@ -16151,8 +16154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:H9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16242,7 +16245,9 @@
       <c r="C8" s="71" t="s">
         <v>5000</v>
       </c>
-      <c r="D8" s="84"/>
+      <c r="D8" s="84" t="s">
+        <v>5057</v>
+      </c>
       <c r="E8" s="85"/>
       <c r="F8" s="85"/>
       <c r="G8" s="85"/>
@@ -16269,7 +16274,7 @@
         <v>5001</v>
       </c>
       <c r="D10" s="73" t="s">
-        <v>5054</v>
+        <v>5049</v>
       </c>
       <c r="E10" s="74"/>
       <c r="F10" s="74"/>
@@ -16297,7 +16302,7 @@
         <v>5002</v>
       </c>
       <c r="D12" s="73" t="s">
-        <v>5053</v>
+        <v>5055</v>
       </c>
       <c r="E12" s="74"/>
       <c r="F12" s="74"/>
@@ -16325,7 +16330,7 @@
         <v>5003</v>
       </c>
       <c r="D14" s="73" t="s">
-        <v>5050</v>
+        <v>5054</v>
       </c>
       <c r="E14" s="74"/>
       <c r="F14" s="74"/>
@@ -16353,7 +16358,7 @@
         <v>5004</v>
       </c>
       <c r="D16" s="73" t="s">
-        <v>5049</v>
+        <v>5052</v>
       </c>
       <c r="E16" s="74"/>
       <c r="F16" s="74"/>
@@ -16381,7 +16386,7 @@
         <v>5005</v>
       </c>
       <c r="D18" s="73" t="s">
-        <v>5052</v>
+        <v>5053</v>
       </c>
       <c r="E18" s="74"/>
       <c r="F18" s="74"/>
@@ -16409,7 +16414,7 @@
         <v>5006</v>
       </c>
       <c r="D20" s="73" t="s">
-        <v>5051</v>
+        <v>5056</v>
       </c>
       <c r="E20" s="74"/>
       <c r="F20" s="74"/>
@@ -16437,7 +16442,7 @@
         <v>5007</v>
       </c>
       <c r="D22" s="73" t="s">
-        <v>5055</v>
+        <v>5058</v>
       </c>
       <c r="E22" s="74"/>
       <c r="F22" s="74"/>
@@ -16465,7 +16470,7 @@
         <v>5008</v>
       </c>
       <c r="D24" s="73" t="s">
-        <v>5058</v>
+        <v>5051</v>
       </c>
       <c r="E24" s="74"/>
       <c r="F24" s="74"/>
@@ -16493,7 +16498,7 @@
         <v>5009</v>
       </c>
       <c r="D26" s="73" t="s">
-        <v>5056</v>
+        <v>5050</v>
       </c>
       <c r="E26" s="74"/>
       <c r="F26" s="74"/>
@@ -16847,6 +16852,7 @@
     <mergeCell ref="C41:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16854,7 +16860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:H19"/>
     </sheetView>
   </sheetViews>
@@ -17042,7 +17048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5011"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -87063,8 +87069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -87141,7 +87147,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="93" t="s">
-        <v>5057</v>
+        <v>5059</v>
       </c>
       <c r="B8" s="91"/>
       <c r="C8" s="91"/>

</xml_diff>

<commit_message>
Complete visualizations and answer remaining questions
</commit_message>
<xml_diff>
--- a/Data Devourers_IIMX.xlsx
+++ b/Data Devourers_IIMX.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5075" uniqueCount="5060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5074" uniqueCount="5059">
   <si>
     <t>ACCT_NUM</t>
   </si>
@@ -15171,39 +15171,36 @@
     <t>Used Regex in re library of Python and Pandas library for further processing to parse the required words. Regex code used to parse all the statements being - "[A-Z].+-Initial Level(.+)". Using this command - It obtained all the keywords from the customer statement seperated by "-". Then further split the string with delimiter "-", to obtain all the keywords in the list. Then, grouped the whole dataframe on the basis of accounts and took union of all those list (in same accounts as same person could do complaint more than once). Next, looped over the grouped dataframe (Used Apply method in Pandas) to change the elements in lists to either - "operation" (for Operation Capabilities), "payment" (for Payment Settlement), "utilit" (for Utilities/ Utility), "account" (for Account) ans simultaaneously counting their numbers and incrementing their value in dictionary of these 4 keywords.</t>
   </si>
   <si>
+    <t>Male tend to be more among churners than females.</t>
+  </si>
+  <si>
+    <t>More Churners are from North and East in comparrison to South and West.</t>
+  </si>
+  <si>
+    <t>People with middle lower salaries are most among Churners.</t>
+  </si>
+  <si>
+    <t>People of medium age - (30 - 60) are more among churners.</t>
+  </si>
+  <si>
+    <t>Those who have rented the equipment have more chnce of being Churner</t>
+  </si>
+  <si>
     <t>Those with valid address are more among Churners</t>
   </si>
   <si>
+    <t>Most Churners from Banking, Financial, Academic Sector</t>
+  </si>
+  <si>
     <t>Those with age of home less than 10 years are more among churners than those with age of home &gt; 10</t>
   </si>
   <si>
+    <t>First, we loaded the data in python using Pandas library. Then Seperated the Modelling and validation accounts for all the different data provided - Demo, Call Center, Default, Payment and Use Pattern data. Further we split the modelling data into training andtest dataset as we wanted to test the performance of our model on an untouched dataset. Pre-Processing :                             
+1. First took important featues from demographic data - Gender, Region, Age, Salary Slab, Professional Info, Age of home, Commence Date, Scheme, Churn Date.
+2. Then change feature - Churn date to Churner (0,1) depending on whether that customer left or not.                                                                                                                           3. Data is of year 2015. So changed the feature - "Commence date" to "Loyal Years of customer" whose value being - (2015 - commence year of customer).                                       4. Other features used for modelling from other data frames ( apart from Demographic Dataframe ) are - "Mean Sum paid in last three months", Complaints made in last 3 months - { "operation", "utility", "payment", "account" }. "Num of times customer was defaulter in last 3 months", "Mean Usage hours in last 3 months".                                                            5. Next, out of all these features Gender, Region, Professional Info, Scheme, Complaints (Customer statements) were the Nominal features and needed to modified properly. So new boolean features were formed i.e Region - {"North", "South", "East", "West"}, Gender - {"Male" -1, "female" - 0}, Complaints - {"operation", "utility", "payment", "account"}, Similarly for schemes and Prof Info also.                                                                                                                                                                                                                                                                   6. Out of all these correlation of these feature were checked to deal with curse of dimensionality. 2 features - "Average hours consumed" and 'Average payment made in last 3 months" were highly correlated. We just used "Average Payment made in last 3 months".                                                                                                                                                 7. We were left with 38 features + "Churner" + "Account Number". Next step we used was to deal with missing values. We imputed them using median.                                             Modelling :                                                                                                                                                                                                                                                                                  1. We now we have got 38 features and 1 target varible - "Churner" -  {0 - Non Churner, 1 - Churner}.                                                                                                                              2. We first used different machine learnng models - KNN, Logistic Regression, SVM - {RBF, Linear, Sigmoid}, Random Forest, Neural Networks. We made use K-Cross validation on our Training set with K = 10 to chose between different hyperparameters of different models with metric being AUC ( of ROC).                                                                                            3. Finally we tested the performance of these models with best hyperparameters on our hold out test set on the basis of AUC again.                                                                           4. Only Logistic Regression and Neural Networks performed quite well with AUC ~ 0.71.                                                                                                                                                     5. We calculated their probability of belonging to class - 1 through predefined functions in scikit learn library of Python. Next we had to chose a threshold. Clearly we want our sensitivity to be high and can somewhat compromise on specificity (but still not too low) because we want to focus on Churners and try to hold them with us. So we chosed the threshold based on maximum F1-Score.                                                                                                                                                                                                                               6. We then finally pre-processed our validation dataset as mentioned above and applied the models - Neural Network and Logistic Regression. My solution is on the basis of Neural Networks as it provied us with more number of churners and is somewhat more complicated than logistic regression.                                                                                      Tools : - Python ( Pandas - Data Processing, sklearn - ML, matplotlib - visualizations, Numpy - Basic array operations ), Excel ( Basic Understanding (Solution 1) and visualizations )</t>
+  </si>
+  <si>
     <t>Assuming average age of marriage being 25, Married people are more among churners.</t>
-  </si>
-  <si>
-    <t>Male tend to be more among churners than females. But propotion of females who are Churner is more than males.</t>
-  </si>
-  <si>
-    <t>Most Churners are in age group of 50-60. But Maximum proportion of Churners in a particular age group is in 10-20.</t>
-  </si>
-  <si>
-    <t>More Churners are from North and East in comparison to South and West.</t>
-  </si>
-  <si>
-    <t>Those who have rented the equipment are more among Churners</t>
-  </si>
-  <si>
-    <t>Churners are most among those with salary range - [0,4] followed by [5-9] which is followed by [10-13]</t>
-  </si>
-  <si>
-    <t>Proportion of Churners is more among those with status - Closed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customers from Banking and Finance make upto 75% of Churners. </t>
-  </si>
-  <si>
-    <t>First, we loaded the data in python using Pandas library. Then Seperated the Modelling and validation accounts for all the different data provided - Demo, Call Center, Default, Payment and Use Pattern data. Further we split the modelling data into training and test dataset as we wanted to test the performance of our model on an untouched dataset. Pre-Processing :                             
-1. First took important featues from demographic data - Gender, Region, Age, Salary Slab, Professional Info, Age of home, Commence Date, Scheme, Churn Date.
-2. Then change feature - Churn date to Churner (0,1) depending on whether that customer left or not.                                                                                                                           3. Data is of year 2015. So changed the feature - "Commence date" to "Loyal Years of customer" whose value being - (2015 - commence year of customer).                                       4. Other features used for modelling from other data frames ( apart from Demographic Dataframe ) are - "Mean Sum paid in last three months", Complaints made in last 3 months - { "operation", "utility", "payment", "account" }. "Num of times customer was defaulter in last 3 months", "Mean Usage hours in last 3 months".                                                            5. Next, out of all these features Gender, Region, Professional Info, Scheme, Complaints (Customer statements) were the Nominal features and needed to modified properly. So new boolean features were formed i.e Region - {"North", "South", "East", "West"}, Gender - {"Male" -1, "female" - 0}, Complaints - {"operation", "utility", "payment", "account"}, Similarly for schemes and Prof Info also.                                                                                                                                                                                                                                                                   6. Out of all these correlation of these feature were checked to deal with curse of dimensionality. 2 features - "Average hours consumed" and 'Average payment made in last 3 months" were highly correlated. We just used "Average Payment made in last 3 months".                                                                                                                                                 7. We were left with 38 features + "Churner" + "Account Number". Next step we used was to deal with missing values. We imputed them using median.                                             Modelling :                                                                                                                                                                                                                                                                                  1. We now we have got 38 features and 1 target varible - "Churner" -  {0 - Non Churner, 1 - Churner}.                                                                                                                              2. We first used different machine learnng models - KNN, Logistic Regression, SVM - {RBF, Linear, Sigmoid}, Random Forest, Neural Networks. We made use of K-Cross validation on our Training set with K = 10 to chose between different hyperparameters of different models with metric being AUC ( of ROC).                                                                                            3. Finally we tested the performance of these models with best hyperparameters on our hold out test set on the basis of AUC again.                                                                           4. Only Logistic Regression and Neural Networks performed well enough with AUC ~ 0.71.                                                                                                                                                     5. We calculated their probability of belonging to class - 1 through predefined functions in scikit learn library of Python. Next we had to chose a threshold. Clearly we want our sensitivity to be high and can somewhat compromise on specificity (but still not too low) because we want to focus on Churners and try to hold them with us. So we chosed the threshold based on maximum F1-Score.                                                                                                                                                                                                                               6. We then finally pre-processed our validation dataset as mentioned above and applied the models - Neural Network and Logistic Regression. My solution is on the basis of 3 layered (2 hidden layers) Neural Networks as it provied us with more number of churners and is somewhat more complicated than logistic regression.                                                                                      Tools : - Python ( Pandas - Data Processing, sklearn - ML, matplotlib - visualizations, Numpy - Basic array operations ), Excel ( Basic Understanding (Solution 1) and visualizations )</t>
   </si>
 </sst>
 </file>
@@ -16154,8 +16151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16245,9 +16242,7 @@
       <c r="C8" s="71" t="s">
         <v>5000</v>
       </c>
-      <c r="D8" s="84" t="s">
-        <v>5057</v>
-      </c>
+      <c r="D8" s="84"/>
       <c r="E8" s="85"/>
       <c r="F8" s="85"/>
       <c r="G8" s="85"/>
@@ -16274,7 +16269,7 @@
         <v>5001</v>
       </c>
       <c r="D10" s="73" t="s">
-        <v>5049</v>
+        <v>5054</v>
       </c>
       <c r="E10" s="74"/>
       <c r="F10" s="74"/>
@@ -16302,7 +16297,7 @@
         <v>5002</v>
       </c>
       <c r="D12" s="73" t="s">
-        <v>5055</v>
+        <v>5053</v>
       </c>
       <c r="E12" s="74"/>
       <c r="F12" s="74"/>
@@ -16330,7 +16325,7 @@
         <v>5003</v>
       </c>
       <c r="D14" s="73" t="s">
-        <v>5054</v>
+        <v>5050</v>
       </c>
       <c r="E14" s="74"/>
       <c r="F14" s="74"/>
@@ -16358,7 +16353,7 @@
         <v>5004</v>
       </c>
       <c r="D16" s="73" t="s">
-        <v>5052</v>
+        <v>5049</v>
       </c>
       <c r="E16" s="74"/>
       <c r="F16" s="74"/>
@@ -16386,7 +16381,7 @@
         <v>5005</v>
       </c>
       <c r="D18" s="73" t="s">
-        <v>5053</v>
+        <v>5052</v>
       </c>
       <c r="E18" s="74"/>
       <c r="F18" s="74"/>
@@ -16414,7 +16409,7 @@
         <v>5006</v>
       </c>
       <c r="D20" s="73" t="s">
-        <v>5056</v>
+        <v>5051</v>
       </c>
       <c r="E20" s="74"/>
       <c r="F20" s="74"/>
@@ -16442,7 +16437,7 @@
         <v>5007</v>
       </c>
       <c r="D22" s="73" t="s">
-        <v>5058</v>
+        <v>5055</v>
       </c>
       <c r="E22" s="74"/>
       <c r="F22" s="74"/>
@@ -16470,7 +16465,7 @@
         <v>5008</v>
       </c>
       <c r="D24" s="73" t="s">
-        <v>5051</v>
+        <v>5058</v>
       </c>
       <c r="E24" s="74"/>
       <c r="F24" s="74"/>
@@ -16498,7 +16493,7 @@
         <v>5009</v>
       </c>
       <c r="D26" s="73" t="s">
-        <v>5050</v>
+        <v>5056</v>
       </c>
       <c r="E26" s="74"/>
       <c r="F26" s="74"/>
@@ -16852,7 +16847,6 @@
     <mergeCell ref="C41:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16860,7 +16854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:H19"/>
     </sheetView>
   </sheetViews>
@@ -17048,7 +17042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5011"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -87069,8 +87063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -87147,7 +87141,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="93" t="s">
-        <v>5059</v>
+        <v>5057</v>
       </c>
       <c r="B8" s="91"/>
       <c r="C8" s="91"/>

</xml_diff>